<commit_message>
Added new datasets and created Polynomial Regression
</commit_message>
<xml_diff>
--- a/transportation.xlsx
+++ b/transportation.xlsx
@@ -1,25 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bandhan\Downloads\machine.learning.project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDBF01A-893D-4B72-9343-D55F6AF4EDA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Sheet1'!$A$3:$O$59</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$3:$O$59</definedName>
   </definedNames>
-  <calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Transportation Emissions by State (1980 - 2017)</t>
   </si>
@@ -203,52 +220,37 @@
   <si>
     <r>
       <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <b val="false"/>
-        <i val="false"/>
-        <vertAlign val="superscript"/>
-        <strike val="false"/>
-        <color rgb="00000000"/>
-        <sz val="9"/>
-        <u val="none"/>
       </rPr>
-      <t xml:space="preserve">1</t>
+      <t>1</t>
     </r>
     <r>
       <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <b val="false"/>
-        <i val="false"/>
-        <strike val="false"/>
-        <color rgb="00000000"/>
-        <sz val="9"/>
-        <u val="none"/>
       </rPr>
       <t xml:space="preserve">For the United States as a whole see, EIA, </t>
     </r>
     <r>
       <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <b val="false"/>
-        <i val="true"/>
-        <strike val="false"/>
-        <color rgb="00000000"/>
-        <sz val="9"/>
-        <u val="none"/>
       </rPr>
-      <t xml:space="preserve">Monthly Energy Review</t>
+      <t>Monthly Energy Review</t>
     </r>
     <r>
       <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <b val="false"/>
-        <i val="false"/>
-        <strike val="false"/>
-        <color rgb="00000000"/>
-        <sz val="9"/>
-        <u val="none"/>
       </rPr>
-      <t xml:space="preserve">, Section 11: Environment.  Differing methodologies between the two data series cause</t>
+      <t>, Section 11: Environment.  Differing methodologies between the two data series cause</t>
     </r>
   </si>
   <si>
@@ -258,79 +260,64 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <sz val="11"/>
-      <b val="0"/>
-      <i val="0"/>
-      <u val="none"/>
-      <strike val="0"/>
-      <color rgb="FF000000"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <sz val="9"/>
-      <b val="0"/>
-      <i val="0"/>
-      <u val="none"/>
-      <strike val="0"/>
-      <color rgb="FF000000"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF0096D7"/>
       <name val="Calibri"/>
-      <sz val="12"/>
-      <b val="1"/>
-      <i val="0"/>
-      <u val="none"/>
-      <strike val="0"/>
-      <color rgb="FF0096D7"/>
     </font>
     <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <sz val="9"/>
-      <b val="1"/>
-      <i val="0"/>
-      <u val="none"/>
-      <strike val="0"/>
-      <color rgb="FF000000"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <sz val="9"/>
-      <b val="0"/>
-      <i val="0"/>
-      <u val="none"/>
-      <strike val="0"/>
-      <color rgb="00000000"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <sz val="11"/>
-      <b val="1"/>
-      <i val="0"/>
-      <u val="none"/>
-      <strike val="0"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="none">
@@ -340,86 +327,105 @@
     </fill>
   </fills>
   <borders count="4">
-    <border/>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="dashed">
         <color rgb="FFBFBFBF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thick">
         <color rgb="FF0096D7"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="medium">
         <color rgb="FF0096D7"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+  <cellXfs count="19">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection locked="false"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection locked="false"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="164" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="3" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="165" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="165" fillId="2" borderId="3" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="165" fillId="2" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -707,36 +713,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AP59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="false" showRowColHeaders="1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="true" style="2"/>
-    <col min="2" max="2" width="9.140625" customWidth="true" style="2"/>
-    <col min="3" max="3" width="9.140625" customWidth="true" style="2"/>
-    <col min="4" max="4" width="9.140625" customWidth="true" style="2"/>
-    <col min="5" max="5" width="9.140625" customWidth="true" style="2"/>
-    <col min="6" max="6" width="9.140625" customWidth="true" style="2"/>
-    <col min="7" max="7" width="9.140625" customWidth="true" style="2"/>
-    <col min="8" max="8" width="9.140625" customWidth="true" style="2"/>
-    <col min="9" max="9" width="9.140625" customWidth="true" style="2"/>
-    <col min="10" max="10" width="9.140625" customWidth="true" style="2"/>
-    <col min="11" max="11" width="9.140625" customWidth="true" style="2"/>
-    <col min="12" max="12" width="9.140625" customWidth="true" style="2"/>
-    <col min="13" max="13" width="9.140625" customWidth="true" style="2"/>
-    <col min="14" max="14" width="10.42578125" customWidth="true" style="2"/>
-    <col min="15" max="15" width="9.42578125" customWidth="true" style="2"/>
-    <col min="16" max="16" width="9.140625" customWidth="true" style="2"/>
+    <col min="1" max="1" width="20.6640625" style="2" customWidth="1"/>
+    <col min="2" max="13" width="9.109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="10.44140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="9.109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" customHeight="1" ht="15.75">
+    <row r="1" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -754,7 +750,7 @@
       <c r="M1" s="1"/>
       <c r="O1" s="3"/>
     </row>
-    <row r="2" spans="1:42">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -770,13 +766,13 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="AN2" s="13" t="s">
+      <c r="AN2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="AO2" s="13"/>
-      <c r="AP2" s="13" t="s"/>
+      <c r="AO2" s="18"/>
+      <c r="AP2" s="12"/>
     </row>
-    <row r="3" spans="1:42" customHeight="1" ht="15.75">
+    <row r="3" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
@@ -900,9 +896,9 @@
       <c r="AO3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="AP3" s="13" t="s"/>
+      <c r="AP3" s="12"/>
     </row>
-    <row r="4" spans="1:42" customHeight="1" ht="12.75">
+    <row r="4" spans="1:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -973,19 +969,19 @@
         <v>31.3</v>
       </c>
       <c r="X4" s="7">
-        <v>33.3</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="Y4" s="7">
-        <v>32.3</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="Z4" s="7">
-        <v>34.8</v>
+        <v>34.799999999999997</v>
       </c>
       <c r="AA4" s="7">
-        <v>34.7</v>
+        <v>34.700000000000003</v>
       </c>
       <c r="AB4" s="7">
-        <v>35.3</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="AC4" s="7">
         <v>35.6</v>
@@ -997,10 +993,10 @@
         <v>31.9</v>
       </c>
       <c r="AF4" s="7">
-        <v>32.2</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="AG4" s="7">
-        <v>32.3</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="AH4" s="7">
         <v>31.8</v>
@@ -1015,20 +1011,20 @@
         <v>32.9</v>
       </c>
       <c r="AL4" s="7">
-        <v>34.7</v>
+        <v>34.700000000000003</v>
       </c>
       <c r="AM4" s="7">
         <v>33.9</v>
       </c>
-      <c r="AN4" s="14">
-        <v>0.3669354838709677</v>
+      <c r="AN4" s="13">
+        <v>0.36693548387096769</v>
       </c>
       <c r="AO4" s="7">
-        <f>(AM4 - B4)</f>
-        <v>-25.5</v>
+        <f t="shared" ref="AO4:AO35" si="0">(AM4 - B4)</f>
+        <v>9.0999999999999979</v>
       </c>
     </row>
-    <row r="5" spans="1:42">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -1042,7 +1038,7 @@
         <v>7.3</v>
       </c>
       <c r="E5" s="7">
-        <v>8.300000000000001</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="F5" s="7">
         <v>10.1</v>
@@ -1111,7 +1107,7 @@
         <v>18.7</v>
       </c>
       <c r="AB5" s="7">
-        <v>18.9</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="AC5" s="7">
         <v>17.8</v>
@@ -1146,15 +1142,15 @@
       <c r="AM5" s="7">
         <v>11.6</v>
       </c>
-      <c r="AN5" s="14">
-        <v>0.8124999999999998</v>
+      <c r="AN5" s="13">
+        <v>0.81249999999999978</v>
       </c>
       <c r="AO5" s="7">
-        <f>(AM5 - B5)</f>
-        <v>1.2</v>
+        <f t="shared" si="0"/>
+        <v>5.1999999999999993</v>
       </c>
     </row>
-    <row r="6" spans="1:42">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -1171,7 +1167,7 @@
         <v>18.5</v>
       </c>
       <c r="F6" s="7">
-        <v>19.6</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="G6" s="7">
         <v>20.5</v>
@@ -1219,34 +1215,34 @@
         <v>31.4</v>
       </c>
       <c r="V6" s="7">
-        <v>32.2</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="W6" s="7">
-        <v>33.3</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="X6" s="7">
         <v>34.1</v>
       </c>
       <c r="Y6" s="7">
-        <v>35.2</v>
+        <v>35.200000000000003</v>
       </c>
       <c r="Z6" s="7">
         <v>36</v>
       </c>
       <c r="AA6" s="7">
-        <v>36.7</v>
+        <v>36.700000000000003</v>
       </c>
       <c r="AB6" s="7">
         <v>37.9</v>
       </c>
       <c r="AC6" s="7">
-        <v>37.3</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="AD6" s="7">
-        <v>34.3</v>
+        <v>34.299999999999997</v>
       </c>
       <c r="AE6" s="7">
-        <v>32.3</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="AF6" s="7">
         <v>31.5</v>
@@ -1272,15 +1268,15 @@
       <c r="AM6" s="7">
         <v>33</v>
       </c>
-      <c r="AN6" s="14">
-        <v>0.7837837837837838</v>
+      <c r="AN6" s="13">
+        <v>0.78378378378378377</v>
       </c>
       <c r="AO6" s="7">
-        <f>(AM6 - B6)</f>
-        <v>8.899999999999999</v>
+        <f t="shared" si="0"/>
+        <v>14.5</v>
       </c>
     </row>
-    <row r="7" spans="1:42">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
@@ -1321,7 +1317,7 @@
         <v>16.2</v>
       </c>
       <c r="N7" s="7">
-        <v>16.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="O7" s="7">
         <v>16.8</v>
@@ -1348,7 +1344,7 @@
         <v>20.8</v>
       </c>
       <c r="W7" s="7">
-        <v>19.6</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="X7" s="7">
         <v>20.2</v>
@@ -1360,10 +1356,10 @@
         <v>20.5</v>
       </c>
       <c r="AA7" s="7">
-        <v>20.4</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="AB7" s="7">
-        <v>20.4</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="AC7" s="7">
         <v>20.8</v>
@@ -1375,10 +1371,10 @@
         <v>19.8</v>
       </c>
       <c r="AF7" s="7">
-        <v>19.6</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="AG7" s="7">
-        <v>19.4</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AH7" s="7">
         <v>18.7</v>
@@ -1393,20 +1389,20 @@
         <v>18.8</v>
       </c>
       <c r="AL7" s="7">
-        <v>19.4</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AM7" s="7">
-        <v>19.4</v>
-      </c>
-      <c r="AN7" s="14">
-        <v>0.3566433566433564</v>
+        <v>19.399999999999999</v>
+      </c>
+      <c r="AN7" s="13">
+        <v>0.35664335664335639</v>
       </c>
       <c r="AO7" s="7">
-        <f>(AM7 - B7)</f>
-        <v>22.2</v>
+        <f t="shared" si="0"/>
+        <v>5.0999999999999979</v>
       </c>
     </row>
-    <row r="8" spans="1:42">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
@@ -1417,10 +1413,10 @@
         <v>169.3</v>
       </c>
       <c r="D8" s="7">
-        <v>160.3</v>
+        <v>160.30000000000001</v>
       </c>
       <c r="E8" s="7">
-        <v>161.8</v>
+        <v>161.80000000000001</v>
       </c>
       <c r="F8" s="7">
         <v>170.2</v>
@@ -1524,15 +1520,15 @@
       <c r="AM8" s="7">
         <v>217.3</v>
       </c>
-      <c r="AN8" s="14">
-        <v>0.2715038033937975</v>
+      <c r="AN8" s="13">
+        <v>0.27150380339379748</v>
       </c>
       <c r="AO8" s="7">
-        <f>(AM8 - B8)</f>
-        <v>-2.899999999999999</v>
+        <f t="shared" si="0"/>
+        <v>46.400000000000006</v>
       </c>
     </row>
-    <row r="9" spans="1:42">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
@@ -1540,7 +1536,7 @@
         <v>17.7</v>
       </c>
       <c r="C9" s="7">
-        <v>17.6</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="D9" s="7">
         <v>18.3</v>
@@ -1552,10 +1548,10 @@
         <v>18.7</v>
       </c>
       <c r="G9" s="7">
-        <v>19.4</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="H9" s="7">
-        <v>19.6</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="I9" s="7">
         <v>19.8</v>
@@ -1564,7 +1560,7 @@
         <v>19.2</v>
       </c>
       <c r="K9" s="7">
-        <v>18.6</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="L9" s="7">
         <v>19</v>
@@ -1650,15 +1646,15 @@
       <c r="AM9" s="7">
         <v>28.6</v>
       </c>
-      <c r="AN9" s="14">
-        <v>0.6158192090395482</v>
+      <c r="AN9" s="13">
+        <v>0.61581920903954823</v>
       </c>
       <c r="AO9" s="7">
-        <f>(AM9 - B9)</f>
-        <v>7.099999999999998</v>
+        <f t="shared" si="0"/>
+        <v>10.900000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:42">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
@@ -1720,10 +1716,10 @@
         <v>15.4</v>
       </c>
       <c r="U10" s="7">
-        <v>16.6</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="V10" s="7">
-        <v>16.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="W10" s="7">
         <v>16.8</v>
@@ -1741,13 +1737,13 @@
         <v>18.2</v>
       </c>
       <c r="AB10" s="7">
-        <v>17.4</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="AC10" s="7">
-        <v>17.4</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="AD10" s="7">
-        <v>16.4</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="AE10" s="7">
         <v>16</v>
@@ -1776,15 +1772,15 @@
       <c r="AM10" s="7">
         <v>15.2</v>
       </c>
-      <c r="AN10" s="14">
+      <c r="AN10" s="13">
         <v>0.1515151515151516</v>
       </c>
       <c r="AO10" s="7">
-        <f>(AM10 - B10)</f>
-        <v>0.2</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:42">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
@@ -1801,10 +1797,10 @@
         <v>4</v>
       </c>
       <c r="F11" s="7">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="G11" s="7">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="H11" s="7">
         <v>4.3</v>
@@ -1813,7 +1809,7 @@
         <v>4.7</v>
       </c>
       <c r="J11" s="7">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="K11" s="7">
         <v>4.7</v>
@@ -1822,13 +1818,13 @@
         <v>4.5</v>
       </c>
       <c r="M11" s="7">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="N11" s="7">
         <v>4.7</v>
       </c>
       <c r="O11" s="7">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="P11" s="7">
         <v>4.5</v>
@@ -1846,22 +1842,22 @@
         <v>4.7</v>
       </c>
       <c r="U11" s="7">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="V11" s="7">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="W11" s="7">
         <v>4.7</v>
       </c>
       <c r="X11" s="7">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="Y11" s="7">
         <v>4.8</v>
       </c>
       <c r="Z11" s="7">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="AA11" s="7">
         <v>5.2</v>
@@ -1873,7 +1869,7 @@
         <v>5.2</v>
       </c>
       <c r="AD11" s="7">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="AE11" s="7">
         <v>4.7</v>
@@ -1882,35 +1878,35 @@
         <v>4.3</v>
       </c>
       <c r="AG11" s="7">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="AH11" s="7">
         <v>4.2</v>
       </c>
       <c r="AI11" s="7">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="AJ11" s="7">
         <v>4.2</v>
       </c>
       <c r="AK11" s="7">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="AL11" s="7">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="AM11" s="7">
         <v>4.7</v>
       </c>
-      <c r="AN11" s="14">
-        <v>0.2051282051282053</v>
+      <c r="AN11" s="13">
+        <v>0.20512820512820529</v>
       </c>
       <c r="AO11" s="7">
-        <f>(AM11 - B11)</f>
-        <v>-2.1</v>
+        <f t="shared" si="0"/>
+        <v>0.80000000000000027</v>
       </c>
     </row>
-    <row r="12" spans="1:42">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>14</v>
       </c>
@@ -2002,13 +1998,13 @@
         <v>1</v>
       </c>
       <c r="AE12" s="7">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AF12" s="7">
         <v>1</v>
       </c>
       <c r="AG12" s="7">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AH12" s="7">
         <v>1</v>
@@ -2017,10 +2013,10 @@
         <v>1</v>
       </c>
       <c r="AJ12" s="7">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AK12" s="7">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AL12" s="7">
         <v>1.2</v>
@@ -2028,15 +2024,15 @@
       <c r="AM12" s="7">
         <v>1</v>
       </c>
-      <c r="AN12" s="14">
-        <v>-0.4736842105263158</v>
+      <c r="AN12" s="13">
+        <v>-0.47368421052631582</v>
       </c>
       <c r="AO12" s="7">
-        <f>(AM12 - B12)</f>
-        <v>-0.3</v>
+        <f t="shared" si="0"/>
+        <v>-0.89999999999999991</v>
       </c>
     </row>
-    <row r="13" spans="1:42">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
@@ -2047,7 +2043,7 @@
         <v>68.2</v>
       </c>
       <c r="D13" s="7">
-        <v>66.90000000000001</v>
+        <v>66.900000000000006</v>
       </c>
       <c r="E13" s="7">
         <v>66.8</v>
@@ -2056,28 +2052,28 @@
         <v>65.5</v>
       </c>
       <c r="G13" s="7">
-        <v>67.90000000000001</v>
+        <v>67.900000000000006</v>
       </c>
       <c r="H13" s="7">
         <v>71.7</v>
       </c>
       <c r="I13" s="7">
-        <v>76.09999999999999</v>
+        <v>76.099999999999994</v>
       </c>
       <c r="J13" s="7">
-        <v>80.59999999999999</v>
+        <v>80.599999999999994</v>
       </c>
       <c r="K13" s="7">
-        <v>81.40000000000001</v>
+        <v>81.400000000000006</v>
       </c>
       <c r="L13" s="7">
-        <v>81.40000000000001</v>
+        <v>81.400000000000006</v>
       </c>
       <c r="M13" s="7">
-        <v>77.09999999999999</v>
+        <v>77.099999999999994</v>
       </c>
       <c r="N13" s="7">
-        <v>79.90000000000001</v>
+        <v>79.900000000000006</v>
       </c>
       <c r="O13" s="7">
         <v>78.8</v>
@@ -2086,10 +2082,10 @@
         <v>84.2</v>
       </c>
       <c r="Q13" s="7">
-        <v>86.40000000000001</v>
+        <v>86.4</v>
       </c>
       <c r="R13" s="7">
-        <v>87.09999999999999</v>
+        <v>87.1</v>
       </c>
       <c r="S13" s="7">
         <v>90.2</v>
@@ -2098,7 +2094,7 @@
         <v>91.7</v>
       </c>
       <c r="U13" s="7">
-        <v>94.40000000000001</v>
+        <v>94.4</v>
       </c>
       <c r="V13" s="7">
         <v>100.1</v>
@@ -2137,7 +2133,7 @@
         <v>102.4</v>
       </c>
       <c r="AH13" s="7">
-        <v>99.40000000000001</v>
+        <v>99.4</v>
       </c>
       <c r="AI13" s="7">
         <v>100</v>
@@ -2154,15 +2150,15 @@
       <c r="AM13" s="7">
         <v>105.6</v>
       </c>
-      <c r="AN13" s="14">
-        <v>0.5483870967741935</v>
+      <c r="AN13" s="13">
+        <v>0.54838709677419351</v>
       </c>
       <c r="AO13" s="7">
-        <f>(AM13 - B13)</f>
-        <v>17.8</v>
+        <f t="shared" si="0"/>
+        <v>37.399999999999991</v>
       </c>
     </row>
-    <row r="14" spans="1:42">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
@@ -2245,10 +2241,10 @@
         <v>68.8</v>
       </c>
       <c r="AB14" s="7">
-        <v>67.90000000000001</v>
+        <v>67.900000000000006</v>
       </c>
       <c r="AC14" s="7">
-        <v>66.09999999999999</v>
+        <v>66.099999999999994</v>
       </c>
       <c r="AD14" s="7">
         <v>60</v>
@@ -2280,15 +2276,15 @@
       <c r="AM14" s="7">
         <v>57.4</v>
       </c>
-      <c r="AN14" s="14">
-        <v>0.4680306905370843</v>
+      <c r="AN14" s="13">
+        <v>0.46803069053708429</v>
       </c>
       <c r="AO14" s="7">
-        <f>(AM14 - B14)</f>
-        <v>-16</v>
+        <f t="shared" si="0"/>
+        <v>18.299999999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:42">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>17</v>
       </c>
@@ -2305,7 +2301,7 @@
         <v>8.5</v>
       </c>
       <c r="F15" s="7">
-        <v>9.300000000000001</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="G15" s="7">
         <v>10.3</v>
@@ -2341,16 +2337,16 @@
         <v>9.9</v>
       </c>
       <c r="R15" s="7">
-        <v>8.699999999999999</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="S15" s="7">
-        <v>8.300000000000001</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="T15" s="7">
         <v>8.1</v>
       </c>
       <c r="U15" s="7">
-        <v>8.800000000000001</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="V15" s="7">
         <v>9</v>
@@ -2380,7 +2376,7 @@
         <v>9.5</v>
       </c>
       <c r="AE15" s="7">
-        <v>9.300000000000001</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="AF15" s="7">
         <v>9.6</v>
@@ -2401,20 +2397,20 @@
         <v>10.1</v>
       </c>
       <c r="AL15" s="7">
-        <v>10.2</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="AM15" s="7">
-        <v>10.2</v>
-      </c>
-      <c r="AN15" s="14">
-        <v>-0.02857142857142869</v>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="AN15" s="13">
+        <v>-2.8571428571428688E-2</v>
       </c>
       <c r="AO15" s="7">
-        <f>(AM15 - B15)</f>
-        <v>1.4</v>
+        <f t="shared" si="0"/>
+        <v>-0.30000000000000071</v>
       </c>
     </row>
-    <row r="16" spans="1:42">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>18</v>
       </c>
@@ -2473,22 +2469,22 @@
         <v>8.1</v>
       </c>
       <c r="T16" s="7">
-        <v>8.199999999999999</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="U16" s="7">
-        <v>8.699999999999999</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="V16" s="7">
-        <v>8.699999999999999</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="W16" s="7">
         <v>8.5</v>
       </c>
       <c r="X16" s="7">
-        <v>8.699999999999999</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="Y16" s="7">
-        <v>8.300000000000001</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="Z16" s="7">
         <v>8.6</v>
@@ -2497,7 +2493,7 @@
         <v>8.6</v>
       </c>
       <c r="AB16" s="7">
-        <v>9.199999999999999</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="AC16" s="7">
         <v>9.5</v>
@@ -2509,7 +2505,7 @@
         <v>8.5</v>
       </c>
       <c r="AF16" s="7">
-        <v>9.199999999999999</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="AG16" s="7">
         <v>8.9</v>
@@ -2518,10 +2514,10 @@
         <v>9</v>
       </c>
       <c r="AI16" s="7">
-        <v>9.199999999999999</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="AJ16" s="7">
-        <v>9.300000000000001</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="AK16" s="7">
         <v>10.3</v>
@@ -2532,15 +2528,15 @@
       <c r="AM16" s="7">
         <v>10.8</v>
       </c>
-      <c r="AN16" s="14">
-        <v>0.8305084745762712</v>
+      <c r="AN16" s="13">
+        <v>0.83050847457627119</v>
       </c>
       <c r="AO16" s="7">
-        <f>(AM16 - B16)</f>
-        <v>-0.7</v>
+        <f t="shared" si="0"/>
+        <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:42">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>19</v>
       </c>
@@ -2605,7 +2601,7 @@
         <v>64.7</v>
       </c>
       <c r="V17" s="7">
-        <v>66.40000000000001</v>
+        <v>66.400000000000006</v>
       </c>
       <c r="W17" s="7">
         <v>64.2</v>
@@ -2617,13 +2613,13 @@
         <v>65</v>
       </c>
       <c r="Z17" s="7">
-        <v>68.59999999999999</v>
+        <v>68.599999999999994</v>
       </c>
       <c r="AA17" s="7">
-        <v>76.09999999999999</v>
+        <v>76.099999999999994</v>
       </c>
       <c r="AB17" s="7">
-        <v>72.40000000000001</v>
+        <v>72.400000000000006</v>
       </c>
       <c r="AC17" s="7">
         <v>72.3</v>
@@ -2632,13 +2628,13 @@
         <v>68.2</v>
       </c>
       <c r="AE17" s="7">
-        <v>66.59999999999999</v>
+        <v>66.599999999999994</v>
       </c>
       <c r="AF17" s="7">
-        <v>65.40000000000001</v>
+        <v>65.400000000000006</v>
       </c>
       <c r="AG17" s="7">
-        <v>64.90000000000001</v>
+        <v>64.900000000000006</v>
       </c>
       <c r="AH17" s="7">
         <v>62.9</v>
@@ -2650,23 +2646,23 @@
         <v>65</v>
       </c>
       <c r="AK17" s="7">
-        <v>67.90000000000001</v>
+        <v>67.900000000000006</v>
       </c>
       <c r="AL17" s="7">
         <v>68.2</v>
       </c>
       <c r="AM17" s="7">
-        <v>68.40000000000001</v>
-      </c>
-      <c r="AN17" s="14">
-        <v>0.1813471502590676</v>
+        <v>68.400000000000006</v>
+      </c>
+      <c r="AN17" s="13">
+        <v>0.18134715025906761</v>
       </c>
       <c r="AO17" s="7">
-        <f>(AM17 - B17)</f>
-        <v>-13.7</v>
+        <f t="shared" si="0"/>
+        <v>10.500000000000007</v>
       </c>
     </row>
-    <row r="18" spans="1:42">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>20</v>
       </c>
@@ -2683,7 +2679,7 @@
         <v>30.7</v>
       </c>
       <c r="F18" s="7">
-        <v>35.8</v>
+        <v>35.799999999999997</v>
       </c>
       <c r="G18" s="7">
         <v>36.4</v>
@@ -2692,13 +2688,13 @@
         <v>38.6</v>
       </c>
       <c r="I18" s="7">
-        <v>40.3</v>
+        <v>40.299999999999997</v>
       </c>
       <c r="J18" s="7">
-        <v>39.2</v>
+        <v>39.200000000000003</v>
       </c>
       <c r="K18" s="7">
-        <v>40.2</v>
+        <v>40.200000000000003</v>
       </c>
       <c r="L18" s="7">
         <v>40.6</v>
@@ -2758,7 +2754,7 @@
         <v>41.3</v>
       </c>
       <c r="AE18" s="7">
-        <v>39.8</v>
+        <v>39.799999999999997</v>
       </c>
       <c r="AF18" s="7">
         <v>41.8</v>
@@ -2767,7 +2763,7 @@
         <v>41.8</v>
       </c>
       <c r="AH18" s="7">
-        <v>40.8</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="AI18" s="7">
         <v>42.5</v>
@@ -2784,15 +2780,15 @@
       <c r="AM18" s="7">
         <v>42</v>
       </c>
-      <c r="AN18" s="14">
-        <v>0.3418530351437699</v>
+      <c r="AN18" s="13">
+        <v>0.34185303514376991</v>
       </c>
       <c r="AO18" s="7">
-        <f>(AM18 - B18)</f>
-        <v>-19.19999999999999</v>
+        <f t="shared" si="0"/>
+        <v>10.7</v>
       </c>
     </row>
-    <row r="19" spans="1:42">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>21</v>
       </c>
@@ -2821,7 +2817,7 @@
         <v>15.6</v>
       </c>
       <c r="J19" s="7">
-        <v>16.1</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="K19" s="7">
         <v>16.2</v>
@@ -2842,28 +2838,28 @@
         <v>17</v>
       </c>
       <c r="Q19" s="7">
-        <v>17.6</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="R19" s="7">
-        <v>18.9</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="S19" s="7">
-        <v>18.4</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="T19" s="7">
         <v>19</v>
       </c>
       <c r="U19" s="7">
-        <v>18.9</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="V19" s="7">
-        <v>18.6</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="W19" s="7">
         <v>18.5</v>
       </c>
       <c r="X19" s="7">
-        <v>19.1</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="Y19" s="7">
         <v>19.3</v>
@@ -2893,7 +2889,7 @@
         <v>20.8</v>
       </c>
       <c r="AH19" s="7">
-        <v>19.9</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="AI19" s="7">
         <v>20.3</v>
@@ -2910,62 +2906,62 @@
       <c r="AM19" s="7">
         <v>20.3</v>
       </c>
-      <c r="AN19" s="14">
-        <v>0.2155688622754492</v>
+      <c r="AN19" s="13">
+        <v>0.21556886227544919</v>
       </c>
       <c r="AO19" s="7">
-        <f>(AM19 - B19)</f>
-        <v>6.600000000000001</v>
+        <f t="shared" si="0"/>
+        <v>3.6000000000000014</v>
       </c>
     </row>
-    <row r="20" spans="1:42">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="7">
-        <v>18.9</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="C20" s="7">
         <v>18</v>
       </c>
       <c r="D20" s="7">
-        <v>17.4</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="E20" s="7">
-        <v>16.9</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="F20" s="7">
         <v>17.3</v>
       </c>
       <c r="G20" s="7">
-        <v>18.1</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="H20" s="7">
-        <v>18.6</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="I20" s="7">
-        <v>19.1</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="J20" s="7">
         <v>20</v>
       </c>
       <c r="K20" s="7">
-        <v>19.4</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="L20" s="7">
-        <v>19.1</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="M20" s="7">
-        <v>17.9</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="N20" s="7">
-        <v>17.6</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="O20" s="7">
-        <v>17.9</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="P20" s="7">
-        <v>16.9</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="Q20" s="7">
         <v>18.8</v>
@@ -2977,13 +2973,13 @@
         <v>18.5</v>
       </c>
       <c r="T20" s="7">
-        <v>18.6</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="U20" s="7">
-        <v>19.6</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="V20" s="7">
-        <v>18.6</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="W20" s="7">
         <v>17.3</v>
@@ -2995,7 +2991,7 @@
         <v>19.5</v>
       </c>
       <c r="Z20" s="7">
-        <v>18.9</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="AA20" s="7">
         <v>17.7</v>
@@ -3007,19 +3003,19 @@
         <v>19.2</v>
       </c>
       <c r="AD20" s="7">
-        <v>18.6</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="AE20" s="7">
         <v>19.3</v>
       </c>
       <c r="AF20" s="7">
-        <v>19.1</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="AG20" s="7">
         <v>18.5</v>
       </c>
       <c r="AH20" s="7">
-        <v>18.4</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="AI20" s="7">
         <v>19.5</v>
@@ -3031,20 +3027,20 @@
         <v>19</v>
       </c>
       <c r="AL20" s="7">
-        <v>18.6</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="AM20" s="7">
-        <v>18.1</v>
-      </c>
-      <c r="AN20" s="14">
-        <v>-0.04232804232804221</v>
+        <v>18.100000000000001</v>
+      </c>
+      <c r="AN20" s="13">
+        <v>-4.2328042328042208E-2</v>
       </c>
       <c r="AO20" s="7">
-        <f>(AM20 - B20)</f>
-        <v>2.699999999999999</v>
+        <f t="shared" si="0"/>
+        <v>-0.79999999999999716</v>
       </c>
     </row>
-    <row r="21" spans="1:42">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>23</v>
       </c>
@@ -3115,7 +3111,7 @@
         <v>31.7</v>
       </c>
       <c r="X21" s="7">
-        <v>32.7</v>
+        <v>32.700000000000003</v>
       </c>
       <c r="Y21" s="7">
         <v>31.4</v>
@@ -3124,7 +3120,7 @@
         <v>34.1</v>
       </c>
       <c r="AA21" s="7">
-        <v>33.2</v>
+        <v>33.200000000000003</v>
       </c>
       <c r="AB21" s="7">
         <v>33</v>
@@ -3160,17 +3156,17 @@
         <v>32</v>
       </c>
       <c r="AM21" s="7">
-        <v>32.3</v>
-      </c>
-      <c r="AN21" s="14">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="AN21" s="13">
         <v>0.4229074889867841</v>
       </c>
       <c r="AO21" s="7">
-        <f>(AM21 - B21)</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>9.5999999999999979</v>
       </c>
     </row>
-    <row r="22" spans="1:42">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>24</v>
       </c>
@@ -3288,15 +3284,15 @@
       <c r="AM22" s="7">
         <v>52.9</v>
       </c>
-      <c r="AN22" s="14">
-        <v>0.1475054229934925</v>
+      <c r="AN22" s="13">
+        <v>0.14750542299349251</v>
       </c>
       <c r="AO22" s="7">
-        <f>(AM22 - B22)</f>
-        <v>13.4</v>
+        <f t="shared" si="0"/>
+        <v>6.7999999999999972</v>
       </c>
     </row>
-    <row r="23" spans="1:42">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>25</v>
       </c>
@@ -3325,13 +3321,13 @@
         <v>7.7</v>
       </c>
       <c r="J23" s="7">
-        <v>8.800000000000001</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="K23" s="7">
         <v>7.9</v>
       </c>
       <c r="L23" s="7">
-        <v>8.199999999999999</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="M23" s="7">
         <v>7.6</v>
@@ -3367,19 +3363,19 @@
         <v>7.6</v>
       </c>
       <c r="X23" s="7">
-        <v>8.699999999999999</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="Y23" s="7">
-        <v>9.300000000000001</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="Z23" s="7">
         <v>8.6</v>
       </c>
       <c r="AA23" s="7">
-        <v>9.300000000000001</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="AB23" s="7">
-        <v>9.300000000000001</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="AC23" s="7">
         <v>8.9</v>
@@ -3394,19 +3390,19 @@
         <v>8.4</v>
       </c>
       <c r="AG23" s="7">
-        <v>8.300000000000001</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="AH23" s="7">
         <v>7.9</v>
       </c>
       <c r="AI23" s="7">
-        <v>8.800000000000001</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="AJ23" s="7">
-        <v>8.800000000000001</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="AK23" s="7">
-        <v>8.800000000000001</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="AL23" s="7">
         <v>8.9</v>
@@ -3414,15 +3410,15 @@
       <c r="AM23" s="7">
         <v>8.4</v>
       </c>
-      <c r="AN23" s="14">
-        <v>0.423728813559322</v>
+      <c r="AN23" s="13">
+        <v>0.42372881355932202</v>
       </c>
       <c r="AO23" s="7">
-        <f>(AM23 - B23)</f>
-        <v>-0.09999999999999998</v>
+        <f t="shared" si="0"/>
+        <v>2.5</v>
       </c>
     </row>
-    <row r="24" spans="1:42">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>26</v>
       </c>
@@ -3540,15 +3536,15 @@
       <c r="AM24" s="7">
         <v>27.3</v>
       </c>
-      <c r="AN24" s="14">
-        <v>0.1973684210526316</v>
+      <c r="AN24" s="13">
+        <v>0.19736842105263161</v>
       </c>
       <c r="AO24" s="7">
-        <f>(AM24 - B24)</f>
-        <v>-11.7</v>
+        <f t="shared" si="0"/>
+        <v>4.5</v>
       </c>
     </row>
-    <row r="25" spans="1:42">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>27</v>
       </c>
@@ -3625,10 +3621,10 @@
         <v>31.5</v>
       </c>
       <c r="Z25" s="7">
-        <v>33.3</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="AA25" s="7">
-        <v>33.7</v>
+        <v>33.700000000000003</v>
       </c>
       <c r="AB25" s="7">
         <v>32.6</v>
@@ -3666,15 +3662,15 @@
       <c r="AM25" s="7">
         <v>30.6</v>
       </c>
-      <c r="AN25" s="14">
-        <v>0.204724409448819</v>
+      <c r="AN25" s="13">
+        <v>0.20472440944881901</v>
       </c>
       <c r="AO25" s="7">
-        <f>(AM25 - B25)</f>
-        <v>-0.9000000000000001</v>
+        <f t="shared" si="0"/>
+        <v>5.2000000000000028</v>
       </c>
     </row>
-    <row r="26" spans="1:42">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>28</v>
       </c>
@@ -3685,7 +3681,7 @@
         <v>42.2</v>
       </c>
       <c r="D26" s="7">
-        <v>39.7</v>
+        <v>39.700000000000003</v>
       </c>
       <c r="E26" s="7">
         <v>40.1</v>
@@ -3792,15 +3788,15 @@
       <c r="AM26" s="7">
         <v>49.5</v>
       </c>
-      <c r="AN26" s="14">
+      <c r="AN26" s="13">
         <v>0.1327231121281465</v>
       </c>
       <c r="AO26" s="7">
-        <f>(AM26 - B26)</f>
-        <v>-23.2</v>
+        <f t="shared" si="0"/>
+        <v>5.7999999999999972</v>
       </c>
     </row>
-    <row r="27" spans="1:42">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>29</v>
       </c>
@@ -3865,7 +3861,7 @@
         <v>33.4</v>
       </c>
       <c r="V27" s="7">
-        <v>34.7</v>
+        <v>34.700000000000003</v>
       </c>
       <c r="W27" s="7">
         <v>33.9</v>
@@ -3877,19 +3873,19 @@
         <v>34.5</v>
       </c>
       <c r="Z27" s="7">
-        <v>35.7</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="AA27" s="7">
-        <v>36.2</v>
+        <v>36.200000000000003</v>
       </c>
       <c r="AB27" s="7">
-        <v>35.7</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="AC27" s="7">
-        <v>35.8</v>
+        <v>35.799999999999997</v>
       </c>
       <c r="AD27" s="7">
-        <v>33.8</v>
+        <v>33.799999999999997</v>
       </c>
       <c r="AE27" s="7">
         <v>31.4</v>
@@ -3918,26 +3914,26 @@
       <c r="AM27" s="7">
         <v>30.8</v>
       </c>
-      <c r="AN27" s="14">
-        <v>0.3162393162393164</v>
+      <c r="AN27" s="13">
+        <v>0.31623931623931639</v>
       </c>
       <c r="AO27" s="7">
-        <f>(AM27 - B27)</f>
-        <v>1.900000000000002</v>
+        <f t="shared" si="0"/>
+        <v>7.4000000000000021</v>
       </c>
     </row>
-    <row r="28" spans="1:42">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B28" s="7">
-        <v>18.1</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="C28" s="7">
         <v>17.8</v>
       </c>
       <c r="D28" s="7">
-        <v>17.4</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="E28" s="7">
         <v>16.8</v>
@@ -3946,13 +3942,13 @@
         <v>16.8</v>
       </c>
       <c r="G28" s="7">
-        <v>17.4</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="H28" s="7">
         <v>18.8</v>
       </c>
       <c r="I28" s="7">
-        <v>20.4</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="J28" s="7">
         <v>21.5</v>
@@ -3961,7 +3957,7 @@
         <v>20</v>
       </c>
       <c r="L28" s="7">
-        <v>20.1</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="M28" s="7">
         <v>22</v>
@@ -4044,15 +4040,15 @@
       <c r="AM28" s="7">
         <v>30.3</v>
       </c>
-      <c r="AN28" s="14">
-        <v>0.6740331491712706</v>
+      <c r="AN28" s="13">
+        <v>0.67403314917127055</v>
       </c>
       <c r="AO28" s="7">
-        <f>(AM28 - B28)</f>
-        <v>-1.9</v>
+        <f t="shared" si="0"/>
+        <v>12.2</v>
       </c>
     </row>
-    <row r="29" spans="1:42">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>31</v>
       </c>
@@ -4093,13 +4089,13 @@
         <v>33.5</v>
       </c>
       <c r="N29" s="7">
-        <v>34.7</v>
+        <v>34.700000000000003</v>
       </c>
       <c r="O29" s="7">
-        <v>35.7</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="P29" s="7">
-        <v>36.7</v>
+        <v>36.700000000000003</v>
       </c>
       <c r="Q29" s="7">
         <v>38.1</v>
@@ -4120,10 +4116,10 @@
         <v>39.1</v>
       </c>
       <c r="W29" s="7">
-        <v>39.3</v>
+        <v>39.299999999999997</v>
       </c>
       <c r="X29" s="7">
-        <v>40.2</v>
+        <v>40.200000000000003</v>
       </c>
       <c r="Y29" s="7">
         <v>41.7</v>
@@ -4153,13 +4149,13 @@
         <v>37.9</v>
       </c>
       <c r="AH29" s="7">
-        <v>36.7</v>
+        <v>36.700000000000003</v>
       </c>
       <c r="AI29" s="7">
         <v>37.1</v>
       </c>
       <c r="AJ29" s="7">
-        <v>37.7</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="AK29" s="7">
         <v>37.5</v>
@@ -4170,15 +4166,15 @@
       <c r="AM29" s="7">
         <v>37.5</v>
       </c>
-      <c r="AN29" s="14">
-        <v>0.2886597938144329</v>
+      <c r="AN29" s="13">
+        <v>0.28865979381443291</v>
       </c>
       <c r="AO29" s="7">
-        <f>(AM29 - B29)</f>
-        <v>18</v>
+        <f t="shared" si="0"/>
+        <v>8.3999999999999986</v>
       </c>
     </row>
-    <row r="30" spans="1:42">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>32</v>
       </c>
@@ -4258,7 +4254,7 @@
         <v>7.7</v>
       </c>
       <c r="AA30" s="7">
-        <v>8.199999999999999</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="AB30" s="7">
         <v>8.5</v>
@@ -4296,15 +4292,15 @@
       <c r="AM30" s="7">
         <v>8</v>
       </c>
-      <c r="AN30" s="14">
-        <v>0.2698412698412698</v>
+      <c r="AN30" s="13">
+        <v>0.26984126984126983</v>
       </c>
       <c r="AO30" s="7">
-        <f>(AM30 - B30)</f>
-        <v>9.300000000000001</v>
+        <f t="shared" si="0"/>
+        <v>1.7000000000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:42">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>33</v>
       </c>
@@ -4312,7 +4308,7 @@
         <v>9.9</v>
       </c>
       <c r="C31" s="7">
-        <v>9.199999999999999</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="D31" s="7">
         <v>9.4</v>
@@ -4321,16 +4317,16 @@
         <v>10</v>
       </c>
       <c r="F31" s="7">
-        <v>9.800000000000001</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="G31" s="7">
-        <v>9.699999999999999</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="H31" s="7">
-        <v>9.800000000000001</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="I31" s="7">
-        <v>10.2</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="J31" s="7">
         <v>11.1</v>
@@ -4342,7 +4338,7 @@
         <v>10.4</v>
       </c>
       <c r="M31" s="7">
-        <v>10.2</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="N31" s="7">
         <v>10.5</v>
@@ -4422,29 +4418,29 @@
       <c r="AM31" s="7">
         <v>13.9</v>
       </c>
-      <c r="AN31" s="14">
-        <v>0.404040404040404</v>
+      <c r="AN31" s="13">
+        <v>0.40404040404040398</v>
       </c>
       <c r="AO31" s="7">
-        <f>(AM31 - B31)</f>
-        <v>13.5</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:42">
+    <row r="32" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B32" s="7">
-        <v>8.300000000000001</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="C32" s="7">
-        <v>8.199999999999999</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="D32" s="7">
         <v>8.1</v>
       </c>
       <c r="E32" s="7">
-        <v>8.199999999999999</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="F32" s="7">
         <v>7.8</v>
@@ -4453,13 +4449,13 @@
         <v>7.9</v>
       </c>
       <c r="H32" s="7">
-        <v>8.199999999999999</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I32" s="7">
         <v>9</v>
       </c>
       <c r="J32" s="7">
-        <v>9.300000000000001</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="K32" s="7">
         <v>9.4</v>
@@ -4468,7 +4464,7 @@
         <v>9.4</v>
       </c>
       <c r="M32" s="7">
-        <v>9.800000000000001</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="N32" s="7">
         <v>10</v>
@@ -4548,20 +4544,20 @@
       <c r="AM32" s="7">
         <v>15.5</v>
       </c>
-      <c r="AN32" s="14">
+      <c r="AN32" s="13">
         <v>0.8674698795180722</v>
       </c>
       <c r="AO32" s="7">
-        <f>(AM32 - B32)</f>
-        <v>-6.1</v>
+        <f t="shared" si="0"/>
+        <v>7.1999999999999993</v>
       </c>
     </row>
-    <row r="33" spans="1:42">
+    <row r="33" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B33" s="7">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C33" s="7">
         <v>4</v>
@@ -4570,16 +4566,16 @@
         <v>4</v>
       </c>
       <c r="E33" s="7">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="F33" s="7">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="G33" s="7">
         <v>4.5</v>
       </c>
       <c r="H33" s="7">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I33" s="7">
         <v>5.3</v>
@@ -4674,20 +4670,20 @@
       <c r="AM33" s="7">
         <v>6.8</v>
       </c>
-      <c r="AN33" s="14">
+      <c r="AN33" s="13">
         <v>0.6585365853658538</v>
       </c>
       <c r="AO33" s="7">
-        <f>(AM33 - B33)</f>
-        <v>-2.4</v>
+        <f t="shared" si="0"/>
+        <v>2.7</v>
       </c>
     </row>
-    <row r="34" spans="1:42">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>36</v>
       </c>
       <c r="B34" s="7">
-        <v>40.8</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="C34" s="7">
         <v>44.3</v>
@@ -4765,10 +4761,10 @@
         <v>69.2</v>
       </c>
       <c r="AB34" s="7">
-        <v>68.40000000000001</v>
+        <v>68.400000000000006</v>
       </c>
       <c r="AC34" s="7">
-        <v>71.90000000000001</v>
+        <v>71.900000000000006</v>
       </c>
       <c r="AD34" s="7">
         <v>72.8</v>
@@ -4800,15 +4796,15 @@
       <c r="AM34" s="7">
         <v>53.3</v>
       </c>
-      <c r="AN34" s="14">
-        <v>0.3063725490196079</v>
+      <c r="AN34" s="13">
+        <v>0.30637254901960792</v>
       </c>
       <c r="AO34" s="7">
-        <f>(AM34 - B34)</f>
-        <v>-4.800000000000001</v>
+        <f t="shared" si="0"/>
+        <v>12.5</v>
       </c>
     </row>
-    <row r="35" spans="1:42">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>37</v>
       </c>
@@ -4825,7 +4821,7 @@
         <v>10.7</v>
       </c>
       <c r="F35" s="7">
-        <v>9.800000000000001</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="G35" s="7">
         <v>11.1</v>
@@ -4926,15 +4922,15 @@
       <c r="AM35" s="7">
         <v>15</v>
       </c>
-      <c r="AN35" s="14">
-        <v>0.271186440677966</v>
+      <c r="AN35" s="13">
+        <v>0.27118644067796599</v>
       </c>
       <c r="AO35" s="7">
-        <f>(AM35 - B35)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.1999999999999993</v>
       </c>
     </row>
-    <row r="36" spans="1:42">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
         <v>38</v>
       </c>
@@ -4990,7 +4986,7 @@
         <v>65.7</v>
       </c>
       <c r="S36" s="7">
-        <v>65.59999999999999</v>
+        <v>65.599999999999994</v>
       </c>
       <c r="T36" s="7">
         <v>66</v>
@@ -4999,19 +4995,19 @@
         <v>66.5</v>
       </c>
       <c r="V36" s="7">
-        <v>66.90000000000001</v>
+        <v>66.900000000000006</v>
       </c>
       <c r="W36" s="7">
         <v>66.7</v>
       </c>
       <c r="X36" s="7">
-        <v>68.40000000000001</v>
+        <v>68.400000000000006</v>
       </c>
       <c r="Y36" s="7">
         <v>73.2</v>
       </c>
       <c r="Z36" s="7">
-        <v>74.90000000000001</v>
+        <v>74.900000000000006</v>
       </c>
       <c r="AA36" s="7">
         <v>73.2</v>
@@ -5020,7 +5016,7 @@
         <v>74.2</v>
       </c>
       <c r="AC36" s="7">
-        <v>73.59999999999999</v>
+        <v>73.599999999999994</v>
       </c>
       <c r="AD36" s="7">
         <v>73</v>
@@ -5035,13 +5031,13 @@
         <v>65.7</v>
       </c>
       <c r="AH36" s="7">
-        <v>68.09999999999999</v>
+        <v>68.099999999999994</v>
       </c>
       <c r="AI36" s="7">
         <v>68.5</v>
       </c>
       <c r="AJ36" s="7">
-        <v>72.90000000000001</v>
+        <v>72.900000000000006</v>
       </c>
       <c r="AK36" s="7">
         <v>71.2</v>
@@ -5052,15 +5048,15 @@
       <c r="AM36" s="7">
         <v>74.7</v>
       </c>
-      <c r="AN36" s="14">
-        <v>0.04184100418410042</v>
+      <c r="AN36" s="13">
+        <v>4.1841004184100417E-2</v>
       </c>
       <c r="AO36" s="7">
-        <f>(AM36 - B36)</f>
-        <v>-27.3</v>
+        <f t="shared" ref="AO36:AO55" si="1">(AM36 - B36)</f>
+        <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:42">
+    <row r="37" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>39</v>
       </c>
@@ -5074,7 +5070,7 @@
         <v>31.8</v>
       </c>
       <c r="E37" s="7">
-        <v>33.3</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="F37" s="7">
         <v>33.9</v>
@@ -5086,7 +5082,7 @@
         <v>36.9</v>
       </c>
       <c r="I37" s="7">
-        <v>38.7</v>
+        <v>38.700000000000003</v>
       </c>
       <c r="J37" s="7">
         <v>40.9</v>
@@ -5095,16 +5091,16 @@
         <v>39.1</v>
       </c>
       <c r="L37" s="7">
-        <v>38.2</v>
+        <v>38.200000000000003</v>
       </c>
       <c r="M37" s="7">
-        <v>37.7</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="N37" s="7">
         <v>38.4</v>
       </c>
       <c r="O37" s="7">
-        <v>39.8</v>
+        <v>39.799999999999997</v>
       </c>
       <c r="P37" s="7">
         <v>41.1</v>
@@ -5178,15 +5174,15 @@
       <c r="AM37" s="7">
         <v>49.2</v>
       </c>
-      <c r="AN37" s="14">
-        <v>0.5619047619047619</v>
+      <c r="AN37" s="13">
+        <v>0.56190476190476191</v>
       </c>
       <c r="AO37" s="7">
-        <f>(AM37 - B37)</f>
-        <v>-25.2</v>
+        <f t="shared" si="1"/>
+        <v>17.700000000000003</v>
       </c>
     </row>
-    <row r="38" spans="1:42">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>40</v>
       </c>
@@ -5200,13 +5196,13 @@
         <v>5.2</v>
       </c>
       <c r="E38" s="7">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="F38" s="7">
         <v>5</v>
       </c>
       <c r="G38" s="7">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="H38" s="7">
         <v>4.7</v>
@@ -5221,22 +5217,22 @@
         <v>4.7</v>
       </c>
       <c r="L38" s="7">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="M38" s="7">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="N38" s="7">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="O38" s="7">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="P38" s="7">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="Q38" s="7">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="R38" s="7">
         <v>5.2</v>
@@ -5296,23 +5292,23 @@
         <v>10</v>
       </c>
       <c r="AK38" s="7">
-        <v>9.199999999999999</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="AL38" s="7">
-        <v>8.300000000000001</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="AM38" s="7">
-        <v>8.800000000000001</v>
-      </c>
-      <c r="AN38" s="14">
-        <v>0.6923076923076923</v>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="AN38" s="13">
+        <v>0.69230769230769229</v>
       </c>
       <c r="AO38" s="7">
-        <f>(AM38 - B38)</f>
-        <v>22.6</v>
+        <f t="shared" si="1"/>
+        <v>3.6000000000000005</v>
       </c>
     </row>
-    <row r="39" spans="1:42">
+    <row r="39" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>41</v>
       </c>
@@ -5383,13 +5379,13 @@
         <v>68</v>
       </c>
       <c r="X39" s="7">
-        <v>68.59999999999999</v>
+        <v>68.599999999999994</v>
       </c>
       <c r="Y39" s="7">
         <v>69.3</v>
       </c>
       <c r="Z39" s="7">
-        <v>70.90000000000001</v>
+        <v>70.900000000000006</v>
       </c>
       <c r="AA39" s="7">
         <v>70.5</v>
@@ -5401,13 +5397,13 @@
         <v>71.5</v>
       </c>
       <c r="AD39" s="7">
-        <v>67.40000000000001</v>
+        <v>67.400000000000006</v>
       </c>
       <c r="AE39" s="7">
         <v>62.8</v>
       </c>
       <c r="AF39" s="7">
-        <v>64.09999999999999</v>
+        <v>64.099999999999994</v>
       </c>
       <c r="AG39" s="7">
         <v>63.4</v>
@@ -5430,15 +5426,15 @@
       <c r="AM39" s="7">
         <v>62.8</v>
       </c>
-      <c r="AN39" s="14">
-        <v>0.1254480286738351</v>
+      <c r="AN39" s="13">
+        <v>0.12544802867383509</v>
       </c>
       <c r="AO39" s="7">
-        <f>(AM39 - B39)</f>
-        <v>-65.3</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:42">
+    <row r="40" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>42</v>
       </c>
@@ -5506,7 +5502,7 @@
         <v>29.9</v>
       </c>
       <c r="W40" s="7">
-        <v>32.8</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="X40" s="7">
         <v>30.6</v>
@@ -5545,10 +5541,10 @@
         <v>30.6</v>
       </c>
       <c r="AJ40" s="7">
-        <v>32.7</v>
+        <v>32.700000000000003</v>
       </c>
       <c r="AK40" s="7">
-        <v>32.2</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="AL40" s="7">
         <v>32.5</v>
@@ -5556,15 +5552,15 @@
       <c r="AM40" s="7">
         <v>32.6</v>
       </c>
-      <c r="AN40" s="14">
-        <v>0.516279069767442</v>
+      <c r="AN40" s="13">
+        <v>0.51627906976744198</v>
       </c>
       <c r="AO40" s="7">
-        <f>(AM40 - B40)</f>
-        <v>8.899999999999999</v>
+        <f t="shared" si="1"/>
+        <v>11.100000000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:42">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>43</v>
       </c>
@@ -5572,22 +5568,22 @@
         <v>17</v>
       </c>
       <c r="C41" s="7">
-        <v>17.9</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="D41" s="7">
         <v>18</v>
       </c>
       <c r="E41" s="7">
-        <v>16.9</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="F41" s="7">
-        <v>16.6</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="G41" s="7">
         <v>17.2</v>
       </c>
       <c r="H41" s="7">
-        <v>17.6</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="I41" s="7">
         <v>18.7</v>
@@ -5677,20 +5673,20 @@
         <v>20.3</v>
       </c>
       <c r="AL41" s="7">
-        <v>20.4</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="AM41" s="7">
         <v>20.7</v>
       </c>
-      <c r="AN41" s="14">
+      <c r="AN41" s="13">
         <v>0.2176470588235293</v>
       </c>
       <c r="AO41" s="7">
-        <f>(AM41 - B41)</f>
-        <v>0.7</v>
+        <f t="shared" si="1"/>
+        <v>3.6999999999999993</v>
       </c>
     </row>
-    <row r="42" spans="1:42">
+    <row r="42" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
         <v>44</v>
       </c>
@@ -5752,13 +5748,13 @@
         <v>67.3</v>
       </c>
       <c r="U42" s="7">
-        <v>67.90000000000001</v>
+        <v>67.900000000000006</v>
       </c>
       <c r="V42" s="7">
-        <v>70.09999999999999</v>
+        <v>70.099999999999994</v>
       </c>
       <c r="W42" s="7">
-        <v>69.90000000000001</v>
+        <v>69.900000000000006</v>
       </c>
       <c r="X42" s="7">
         <v>70.3</v>
@@ -5767,7 +5763,7 @@
         <v>69.2</v>
       </c>
       <c r="Z42" s="7">
-        <v>70.90000000000001</v>
+        <v>70.900000000000006</v>
       </c>
       <c r="AA42" s="7">
         <v>72.2</v>
@@ -5808,15 +5804,15 @@
       <c r="AM42" s="7">
         <v>63.8</v>
       </c>
-      <c r="AN42" s="14">
+      <c r="AN42" s="13">
         <v>0.1057192374350087</v>
       </c>
       <c r="AO42" s="7">
-        <f>(AM42 - B42)</f>
-        <v>-88.5</v>
+        <f t="shared" si="1"/>
+        <v>6.0999999999999943</v>
       </c>
     </row>
-    <row r="43" spans="1:42">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
         <v>45</v>
       </c>
@@ -5845,67 +5841,67 @@
         <v>4.3</v>
       </c>
       <c r="J43" s="7">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="K43" s="7">
         <v>4.3</v>
       </c>
       <c r="L43" s="7">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="M43" s="7">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="N43" s="7">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="O43" s="7">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="P43" s="7">
         <v>4</v>
       </c>
       <c r="Q43" s="7">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="R43" s="7">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="S43" s="7">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="T43" s="7">
         <v>4.5</v>
       </c>
       <c r="U43" s="7">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="V43" s="7">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="W43" s="7">
         <v>4.7</v>
       </c>
       <c r="X43" s="7">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="Y43" s="7">
         <v>4.5</v>
       </c>
       <c r="Z43" s="7">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="AA43" s="7">
         <v>4.3</v>
       </c>
       <c r="AB43" s="7">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="AC43" s="7">
         <v>4.3</v>
       </c>
       <c r="AD43" s="7">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="AE43" s="7">
         <v>4.2</v>
@@ -5923,10 +5919,10 @@
         <v>3.9</v>
       </c>
       <c r="AJ43" s="7">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="AK43" s="7">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="AL43" s="7">
         <v>3.8</v>
@@ -5934,15 +5930,15 @@
       <c r="AM43" s="7">
         <v>4</v>
       </c>
-      <c r="AN43" s="14">
-        <v>0.08108108108108092</v>
+      <c r="AN43" s="13">
+        <v>8.1081081081080919E-2</v>
       </c>
       <c r="AO43" s="7">
-        <f>(AM43 - B43)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.29999999999999982</v>
       </c>
     </row>
-    <row r="44" spans="1:42">
+    <row r="44" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
         <v>46</v>
       </c>
@@ -5962,10 +5958,10 @@
         <v>18.7</v>
       </c>
       <c r="G44" s="7">
-        <v>18.9</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="H44" s="7">
-        <v>19.6</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="I44" s="7">
         <v>19.3</v>
@@ -6060,15 +6056,15 @@
       <c r="AM44" s="7">
         <v>33</v>
       </c>
-      <c r="AN44" s="14">
-        <v>0.8644067796610171</v>
+      <c r="AN44" s="13">
+        <v>0.86440677966101709</v>
       </c>
       <c r="AO44" s="7">
-        <f>(AM44 - B44)</f>
-        <v>-4.600000000000001</v>
+        <f t="shared" si="1"/>
+        <v>15.3</v>
       </c>
     </row>
-    <row r="45" spans="1:42">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
         <v>47</v>
       </c>
@@ -6079,22 +6075,22 @@
         <v>4.3</v>
       </c>
       <c r="D45" s="7">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E45" s="7">
         <v>4.2</v>
       </c>
       <c r="F45" s="7">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="G45" s="7">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="H45" s="7">
         <v>4.2</v>
       </c>
       <c r="I45" s="7">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="J45" s="7">
         <v>4.5</v>
@@ -6103,16 +6099,16 @@
         <v>4.5</v>
       </c>
       <c r="L45" s="7">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="M45" s="7">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="N45" s="7">
         <v>5</v>
       </c>
       <c r="O45" s="7">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="P45" s="7">
         <v>5.4</v>
@@ -6186,15 +6182,15 @@
       <c r="AM45" s="7">
         <v>6.6</v>
       </c>
-      <c r="AN45" s="14">
-        <v>0.4666666666666666</v>
+      <c r="AN45" s="13">
+        <v>0.46666666666666662</v>
       </c>
       <c r="AO45" s="7">
-        <f>(AM45 - B45)</f>
-        <v>-0.8999999999999999</v>
+        <f t="shared" si="1"/>
+        <v>2.0999999999999996</v>
       </c>
     </row>
-    <row r="46" spans="1:42">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>48</v>
       </c>
@@ -6223,10 +6219,10 @@
         <v>31.7</v>
       </c>
       <c r="J46" s="7">
-        <v>32.2</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="K46" s="7">
-        <v>33.2</v>
+        <v>33.200000000000003</v>
       </c>
       <c r="L46" s="7">
         <v>32.6</v>
@@ -6253,7 +6249,7 @@
         <v>38.4</v>
       </c>
       <c r="T46" s="7">
-        <v>39.3</v>
+        <v>39.299999999999997</v>
       </c>
       <c r="U46" s="7">
         <v>40.5</v>
@@ -6312,15 +6308,15 @@
       <c r="AM46" s="7">
         <v>43.5</v>
       </c>
-      <c r="AN46" s="14">
-        <v>0.5104166666666665</v>
+      <c r="AN46" s="13">
+        <v>0.51041666666666652</v>
       </c>
       <c r="AO46" s="7">
-        <f>(AM46 - B46)</f>
-        <v>-22.2</v>
+        <f t="shared" si="1"/>
+        <v>14.7</v>
       </c>
     </row>
-    <row r="47" spans="1:42">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>49</v>
       </c>
@@ -6331,7 +6327,7 @@
         <v>130</v>
       </c>
       <c r="D47" s="7">
-        <v>133.8</v>
+        <v>133.80000000000001</v>
       </c>
       <c r="E47" s="7">
         <v>133</v>
@@ -6340,7 +6336,7 @@
         <v>138.5</v>
       </c>
       <c r="G47" s="7">
-        <v>143.3</v>
+        <v>143.30000000000001</v>
       </c>
       <c r="H47" s="7">
         <v>146.9</v>
@@ -6364,13 +6360,13 @@
         <v>153.1</v>
       </c>
       <c r="O47" s="7">
-        <v>151.7</v>
+        <v>151.69999999999999</v>
       </c>
       <c r="P47" s="7">
         <v>155.4</v>
       </c>
       <c r="Q47" s="7">
-        <v>153.2</v>
+        <v>153.19999999999999</v>
       </c>
       <c r="R47" s="7">
         <v>165.8</v>
@@ -6438,15 +6434,15 @@
       <c r="AM47" s="7">
         <v>232</v>
       </c>
-      <c r="AN47" s="14">
-        <v>0.8040435458786936</v>
+      <c r="AN47" s="13">
+        <v>0.80404354587869364</v>
       </c>
       <c r="AO47" s="7">
-        <f>(AM47 - B47)</f>
-        <v>69.99999999999999</v>
+        <f t="shared" si="1"/>
+        <v>103.4</v>
       </c>
     </row>
-    <row r="48" spans="1:42">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
         <v>50</v>
       </c>
@@ -6454,10 +6450,10 @@
         <v>9</v>
       </c>
       <c r="C48" s="7">
-        <v>8.699999999999999</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="D48" s="7">
-        <v>8.699999999999999</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="E48" s="7">
         <v>9</v>
@@ -6478,7 +6474,7 @@
         <v>10.7</v>
       </c>
       <c r="K48" s="7">
-        <v>10.2</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="L48" s="7">
         <v>10.6</v>
@@ -6523,10 +6519,10 @@
         <v>15.8</v>
       </c>
       <c r="Z48" s="7">
-        <v>16.4</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="AA48" s="7">
-        <v>16.6</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="AB48" s="7">
         <v>18.3</v>
@@ -6547,10 +6543,10 @@
         <v>17</v>
       </c>
       <c r="AH48" s="7">
-        <v>16.4</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="AI48" s="7">
-        <v>17.1</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="AJ48" s="7">
         <v>16.8</v>
@@ -6564,15 +6560,15 @@
       <c r="AM48" s="7">
         <v>17.7</v>
       </c>
-      <c r="AN48" s="14">
-        <v>0.9666666666666666</v>
+      <c r="AN48" s="13">
+        <v>0.96666666666666656</v>
       </c>
       <c r="AO48" s="7">
-        <f>(AM48 - B48)</f>
-        <v>10.5</v>
+        <f t="shared" si="1"/>
+        <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="49" spans="1:42">
+    <row r="49" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
         <v>51</v>
       </c>
@@ -6583,7 +6579,7 @@
         <v>2.4</v>
       </c>
       <c r="D49" s="7">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E49" s="7">
         <v>2.4</v>
@@ -6690,15 +6686,15 @@
       <c r="AM49" s="7">
         <v>3.3</v>
       </c>
-      <c r="AN49" s="14">
+      <c r="AN49" s="13">
         <v>0.375</v>
       </c>
       <c r="AO49" s="7">
-        <f>(AM49 - B49)</f>
-        <v>-0.1</v>
+        <f t="shared" si="1"/>
+        <v>0.89999999999999991</v>
       </c>
     </row>
-    <row r="50" spans="1:42">
+    <row r="50" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>52</v>
       </c>
@@ -6730,7 +6726,7 @@
         <v>42.4</v>
       </c>
       <c r="K50" s="7">
-        <v>40.7</v>
+        <v>40.700000000000003</v>
       </c>
       <c r="L50" s="7">
         <v>41.4</v>
@@ -6739,7 +6735,7 @@
         <v>40.5</v>
       </c>
       <c r="N50" s="7">
-        <v>40.3</v>
+        <v>40.299999999999997</v>
       </c>
       <c r="O50" s="7">
         <v>41</v>
@@ -6816,15 +6812,15 @@
       <c r="AM50" s="7">
         <v>47.5</v>
       </c>
-      <c r="AN50" s="14">
+      <c r="AN50" s="13">
         <v>0.3808139534883721</v>
       </c>
       <c r="AO50" s="7">
-        <f>(AM50 - B50)</f>
-        <v>-6.5</v>
+        <f t="shared" si="1"/>
+        <v>13.100000000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:42">
+    <row r="51" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
         <v>53</v>
       </c>
@@ -6847,7 +6843,7 @@
         <v>29.7</v>
       </c>
       <c r="H51" s="7">
-        <v>34.7</v>
+        <v>34.700000000000003</v>
       </c>
       <c r="I51" s="7">
         <v>35.6</v>
@@ -6942,20 +6938,20 @@
       <c r="AM51" s="7">
         <v>47.2</v>
       </c>
-      <c r="AN51" s="14">
-        <v>0.5733333333333335</v>
+      <c r="AN51" s="13">
+        <v>0.57333333333333347</v>
       </c>
       <c r="AO51" s="7">
-        <f>(AM51 - B51)</f>
-        <v>-2.6</v>
+        <f t="shared" si="1"/>
+        <v>17.200000000000003</v>
       </c>
     </row>
-    <row r="52" spans="1:42">
+    <row r="52" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
         <v>54</v>
       </c>
       <c r="B52" s="7">
-        <v>10.2</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="C52" s="7">
         <v>9.9</v>
@@ -6988,7 +6984,7 @@
         <v>10.3</v>
       </c>
       <c r="M52" s="7">
-        <v>10.2</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="N52" s="7">
         <v>11</v>
@@ -7068,15 +7064,15 @@
       <c r="AM52" s="7">
         <v>11.5</v>
       </c>
-      <c r="AN52" s="14">
-        <v>0.1274509803921569</v>
+      <c r="AN52" s="13">
+        <v>0.12745098039215691</v>
       </c>
       <c r="AO52" s="7">
-        <f>(AM52 - B52)</f>
-        <v>-12.3</v>
+        <f t="shared" si="1"/>
+        <v>1.3000000000000007</v>
       </c>
     </row>
-    <row r="53" spans="1:42">
+    <row r="53" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
         <v>55</v>
       </c>
@@ -7194,15 +7190,15 @@
       <c r="AM53" s="7">
         <v>28.8</v>
       </c>
-      <c r="AN53" s="14">
+      <c r="AN53" s="13">
         <v>0.2360515021459226</v>
       </c>
       <c r="AO53" s="7">
-        <f>(AM53 - B53)</f>
-        <v>6.400000000000002</v>
+        <f t="shared" si="1"/>
+        <v>5.5</v>
       </c>
     </row>
-    <row r="54" spans="1:42">
+    <row r="54" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>56</v>
       </c>
@@ -7282,22 +7278,22 @@
         <v>8</v>
       </c>
       <c r="AA54" s="7">
-        <v>8.300000000000001</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="AB54" s="7">
         <v>8.5</v>
       </c>
       <c r="AC54" s="7">
-        <v>8.699999999999999</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="AD54" s="7">
         <v>8.5</v>
       </c>
       <c r="AE54" s="7">
-        <v>8.199999999999999</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="AF54" s="7">
-        <v>8.300000000000001</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="AG54" s="7">
         <v>7.6</v>
@@ -7320,15 +7316,15 @@
       <c r="AM54" s="7">
         <v>7.8</v>
       </c>
-      <c r="AN54" s="14">
-        <v>0.2580645161290323</v>
+      <c r="AN54" s="13">
+        <v>0.25806451612903231</v>
       </c>
       <c r="AO54" s="7">
-        <f>(AM54 - B54)</f>
-        <v>18.7</v>
+        <f t="shared" si="1"/>
+        <v>1.5999999999999996</v>
       </c>
     </row>
-    <row r="55" spans="1:42" customHeight="1" ht="12.75">
+    <row r="55" spans="1:41" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>57</v>
       </c>
@@ -7446,158 +7442,123 @@
       <c r="AM55" s="7">
         <v>1905.1</v>
       </c>
-      <c r="AN55" s="14">
-        <v>0.3629274574331092</v>
+      <c r="AN55" s="13">
+        <v>0.36292745743310922</v>
       </c>
       <c r="AO55" s="7">
-        <f>(AM55 - B55)</f>
-        <v>-124.3</v>
+        <f t="shared" si="1"/>
+        <v>507.29999999999995</v>
       </c>
     </row>
-    <row r="56" spans="1:42" customHeight="1" ht="14.25">
-      <c r="A56" s="11" t="s">
+    <row r="56" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="12"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
-      <c r="G56" s="12"/>
-      <c r="H56" s="12"/>
-      <c r="I56" s="12"/>
-      <c r="J56" s="12"/>
-      <c r="K56" s="12"/>
-      <c r="L56" s="12"/>
-      <c r="M56" s="12"/>
-      <c r="N56" s="12"/>
-      <c r="O56" s="12"/>
-      <c r="P56" s="12" t="s"/>
-      <c r="Q56" s="12" t="s"/>
-      <c r="R56" s="12" t="s"/>
-      <c r="S56" s="12" t="s"/>
-      <c r="T56" s="12" t="s"/>
-      <c r="U56" s="12" t="s"/>
-      <c r="V56" s="12" t="s"/>
-      <c r="W56" s="12" t="s"/>
-      <c r="X56" s="12" t="s"/>
-      <c r="Y56" s="12" t="s"/>
-      <c r="Z56" s="12" t="s"/>
-      <c r="AA56" s="12" t="s"/>
-      <c r="AB56" s="12" t="s"/>
-      <c r="AC56" s="12" t="s"/>
-      <c r="AD56" s="12" t="s"/>
-      <c r="AE56" s="12" t="s"/>
-      <c r="AF56" s="12" t="s"/>
-      <c r="AG56" s="12" t="s"/>
-      <c r="AH56" s="12" t="s"/>
-      <c r="AI56" s="12" t="s"/>
-      <c r="AJ56" s="12" t="s"/>
-      <c r="AK56" s="12" t="s"/>
-      <c r="AL56" s="12" t="s"/>
-      <c r="AM56" s="12" t="s"/>
-      <c r="AN56" s="15" t="s"/>
-      <c r="AO56" s="12" t="s"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="17"/>
+      <c r="J56" s="17"/>
+      <c r="K56" s="17"/>
+      <c r="L56" s="17"/>
+      <c r="M56" s="17"/>
+      <c r="N56" s="17"/>
+      <c r="O56" s="17"/>
+      <c r="P56" s="11"/>
+      <c r="Q56" s="11"/>
+      <c r="R56" s="11"/>
+      <c r="S56" s="11"/>
+      <c r="T56" s="11"/>
+      <c r="U56" s="11"/>
+      <c r="V56" s="11"/>
+      <c r="W56" s="11"/>
+      <c r="X56" s="11"/>
+      <c r="Y56" s="11"/>
+      <c r="Z56" s="11"/>
+      <c r="AA56" s="11"/>
+      <c r="AB56" s="11"/>
+      <c r="AC56" s="11"/>
+      <c r="AD56" s="11"/>
+      <c r="AE56" s="11"/>
+      <c r="AF56" s="11"/>
+      <c r="AG56" s="11"/>
+      <c r="AH56" s="11"/>
+      <c r="AI56" s="11"/>
+      <c r="AJ56" s="11"/>
+      <c r="AK56" s="11"/>
+      <c r="AL56" s="11"/>
+      <c r="AM56" s="11"/>
+      <c r="AN56" s="14"/>
+      <c r="AO56" s="11"/>
     </row>
-    <row r="57" spans="1:42" customHeight="1" ht="10.5">
+    <row r="57" spans="1:41" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="AN57" s="16" t="s"/>
+      <c r="AN57" s="15"/>
     </row>
-    <row r="58" spans="1:42" customHeight="1" ht="14.25">
+    <row r="58" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="10" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:42">
+    <row r="59" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>61</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <mergeCells>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="2">
     <mergeCell ref="A56:O56"/>
     <mergeCell ref="AN2:AO2"/>
   </mergeCells>
-  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait" scale="61" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageSetup scale="61" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:A12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A12"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="false" showRowColHeaders="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="true" style="0"/>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="12" spans="1:1" customHeight="1" ht="50.25"/>
+    <row r="12" ht="50.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:E9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A8:A9"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="false" showRowColHeaders="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="true" style="0"/>
-    <col min="2" max="2" width="15.7109375" customWidth="true" style="0"/>
-    <col min="3" max="3" width="11.7109375" customWidth="true" style="0"/>
-    <col min="4" max="4" width="11.7109375" customWidth="true" style="0"/>
-    <col min="5" max="5" width="10.85546875" customWidth="true" style="0"/>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="1:5" customHeight="1" ht="12.75"/>
-    <row r="9" spans="1:5" customHeight="1" ht="25.5"/>
+    <row r="8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>